<commit_message>
EPBDS-6580 Add support Generics for methods (Support only GenericArrayType and TypeVariable)
</commit_message>
<xml_diff>
--- a/DEV/org.openl.rules/test/rules/binding/AutoCastReturnTypeMethodsTest.xlsx
+++ b/DEV/org.openl.rules/test/rules/binding/AutoCastReturnTypeMethodsTest.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17329"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="17927"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>return flatten(new String[][]{{"1","2","3"},{"1","2","3"}});</t>
   </si>
@@ -35,6 +35,12 @@
   </si>
   <si>
     <t>Datatype MyInt2 &lt;Integer&gt;</t>
+  </si>
+  <si>
+    <t>Method String[][] removeTest()</t>
+  </si>
+  <si>
+    <t>return (String[][])remove(new String[][]{{"1","2","3"},{"3","2","1"}}, 1);</t>
   </si>
 </sst>
 </file>
@@ -489,15 +495,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B6:B7"/>
+  <dimension ref="B6:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:B7"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="45.625" customWidth="1"/>
+    <col min="2" max="2" width="45.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="6" spans="2:2" x14ac:dyDescent="0.25">
@@ -508,6 +514,16 @@
     <row r="7" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B12" s="2" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>
@@ -526,7 +542,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="24.875" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:2" x14ac:dyDescent="0.25">

</xml_diff>